<commit_message>
threading on left pi
</commit_message>
<xml_diff>
--- a/cameras.xlsx
+++ b/cameras.xlsx
@@ -180,7 +180,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -440,11 +439,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1301636432"/>
-        <c:axId val="-1275869632"/>
+        <c:axId val="1214343984"/>
+        <c:axId val="1214346032"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1301636432"/>
+        <c:axId val="1214343984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1920.0"/>
@@ -502,14 +501,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1275869632"/>
+        <c:crossAx val="1214346032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="192.0"/>
         <c:minorUnit val="19.2"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1275869632"/>
+        <c:axId val="1214346032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1080.0"/>
@@ -567,7 +566,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1301636432"/>
+        <c:crossAx val="1214343984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="108.0"/>
@@ -633,7 +632,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1110,11 +1108,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1280917568"/>
-        <c:axId val="-1280655680"/>
+        <c:axId val="1210281040"/>
+        <c:axId val="1210283344"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1280917568"/>
+        <c:axId val="1210281040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1920.0"/>
@@ -1172,14 +1170,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1280655680"/>
+        <c:crossAx val="1210283344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="192.0"/>
         <c:minorUnit val="19.2"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1280655680"/>
+        <c:axId val="1210283344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1080.0"/>
@@ -1237,7 +1235,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1280917568"/>
+        <c:crossAx val="1210281040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="108.0"/>
@@ -2735,10 +2733,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R71"/>
+  <dimension ref="A1:R73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="C65" sqref="C65"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="A72" sqref="A72:D73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4219,137 +4217,158 @@
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A63">
-        <v>-24.588000000000001</v>
+        <v>-3.609</v>
       </c>
       <c r="B63">
-        <v>3.4860000000000002</v>
+        <v>1.5289999999999999</v>
       </c>
       <c r="C63">
-        <v>107.80200000000001</v>
+        <v>35.933999999999997</v>
       </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A64">
-        <v>21.437000000000001</v>
+        <v>0.48599999999999999</v>
       </c>
       <c r="B64">
-        <v>3.3660000000000001</v>
+        <v>1.5269999999999999</v>
       </c>
       <c r="C64">
-        <v>104.08499999999999</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+        <v>40.79</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65">
-        <v>-21.562000000000001</v>
+        <v>-3.6930000000000001</v>
       </c>
       <c r="B65">
-        <v>2.468</v>
+        <v>1.6859999999999999</v>
       </c>
       <c r="C65">
-        <v>95.069000000000003</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+        <v>47.162999999999997</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66">
-        <v>-25.52</v>
+        <v>-10.606999999999999</v>
       </c>
       <c r="B66">
-        <v>2.5499999999999998</v>
+        <v>1.74</v>
       </c>
       <c r="C66">
-        <v>399.13</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+        <v>48.685000000000002</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67">
-        <v>33.96</v>
+        <v>-10.49</v>
       </c>
       <c r="B67">
-        <v>3.23</v>
+        <v>1.82</v>
       </c>
       <c r="C67">
-        <v>427.4</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+        <v>62.884</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68">
+        <v>-9.3119999999999994</v>
+      </c>
+      <c r="B68">
+        <v>-4.0670000000000002</v>
+      </c>
+      <c r="C68">
+        <v>62.884</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69">
         <f>A64-A63</f>
-        <v>46.025000000000006</v>
-      </c>
-      <c r="B68">
-        <f t="shared" ref="B68:C71" si="1">B64-B63</f>
-        <v>-0.12000000000000011</v>
-      </c>
-      <c r="C68">
-        <f t="shared" si="1"/>
-        <v>-3.717000000000013</v>
-      </c>
-      <c r="D68">
-        <f>SQRT((A68^2)+(B68^2)+(C68^2))</f>
-        <v>46.175005295072793</v>
-      </c>
-      <c r="F68">
-        <f>24/28</f>
-        <v>0.8571428571428571</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A69">
-        <f>A65-A64</f>
-        <v>-42.999000000000002</v>
+        <v>4.0949999999999998</v>
       </c>
       <c r="B69">
-        <f t="shared" si="1"/>
-        <v>-0.89800000000000013</v>
+        <f t="shared" ref="B69:C73" si="1">B64-B63</f>
+        <v>-2.0000000000000018E-3</v>
       </c>
       <c r="C69">
         <f t="shared" si="1"/>
-        <v>-9.0159999999999911</v>
+        <v>4.8560000000000016</v>
       </c>
       <c r="D69">
         <f>SQRT((A69^2)+(B69^2)+(C69^2))</f>
-        <v>43.94324363312294</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+        <v>6.3521464876055891</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70">
-        <f>A66-A65</f>
-        <v>-3.9579999999999984</v>
+        <f>A65-A64</f>
+        <v>-4.1790000000000003</v>
       </c>
       <c r="B70">
         <f t="shared" si="1"/>
-        <v>8.1999999999999851E-2</v>
+        <v>0.15900000000000003</v>
       </c>
       <c r="C70">
         <f t="shared" si="1"/>
-        <v>304.06099999999998</v>
+        <v>6.3729999999999976</v>
       </c>
       <c r="D70">
         <f>SQRT((A70^2)+(B70^2)+(C70^2))</f>
-        <v>304.08677085496498</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+        <v>7.6226275653477895</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71">
-        <f>A67-A66</f>
-        <v>59.480000000000004</v>
+        <f>A66-A65</f>
+        <v>-6.9139999999999997</v>
       </c>
       <c r="B71">
         <f t="shared" si="1"/>
-        <v>0.68000000000000016</v>
+        <v>5.4000000000000048E-2</v>
       </c>
       <c r="C71">
         <f t="shared" si="1"/>
-        <v>28.269999999999982</v>
+        <v>1.5220000000000056</v>
       </c>
       <c r="D71">
         <f>SQRT((A71^2)+(B71^2)+(C71^2))</f>
-        <v>65.859894473040256</v>
-      </c>
-      <c r="F71">
-        <f>48/66</f>
-        <v>0.72727272727272729</v>
+        <v>7.0797454756509444</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <f>A67-A66</f>
+        <v>0.1169999999999991</v>
+      </c>
+      <c r="B72">
+        <f t="shared" si="1"/>
+        <v>8.0000000000000071E-2</v>
+      </c>
+      <c r="C72">
+        <f t="shared" si="1"/>
+        <v>14.198999999999998</v>
+      </c>
+      <c r="D72">
+        <f>SQRT((A72^2)+(B72^2)+(C72^2))</f>
+        <v>14.199707391351414</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <f>A68-A67</f>
+        <v>1.1780000000000008</v>
+      </c>
+      <c r="B73">
+        <f t="shared" si="1"/>
+        <v>-5.8870000000000005</v>
+      </c>
+      <c r="C73">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D73">
+        <f>SQRT((A73^2)+(B73^2)+(C73^2))</f>
+        <v>6.0037032738135885</v>
       </c>
     </row>
   </sheetData>

</xml_diff>